<commit_message>
base de donneées pretes
</commit_message>
<xml_diff>
--- a/donne conssessionnaire.xlsx
+++ b/donne conssessionnaire.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elie\Desktop\repertoire_git\BDD_-concessionnaire\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E125B3A-74CD-40DC-B9D8-BC7428C1FE17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05F2F00F-3405-429A-BCED-952295FE81A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="concessionaire" sheetId="1" r:id="rId1"/>
@@ -2920,7 +2920,7 @@
     <numFmt numFmtId="164" formatCode="dd\-mmm\-yyyy"/>
     <numFmt numFmtId="165" formatCode="d\-mmm\-yyyy"/>
     <numFmt numFmtId="166" formatCode="d\-mmmm\-yyyy"/>
-    <numFmt numFmtId="168" formatCode="[$-409]d\-mmm\-yyyy;@"/>
+    <numFmt numFmtId="167" formatCode="[$-409]d\-mmm\-yyyy;@"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -3037,25 +3037,23 @@
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="15" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4603,7 +4601,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+    <sheetView topLeftCell="A33" workbookViewId="0">
       <selection activeCell="F2" sqref="F2:F76"/>
     </sheetView>
   </sheetViews>
@@ -9222,7 +9220,7 @@
       </c>
     </row>
     <row r="135" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="20">
+      <c r="A135" s="19">
         <v>134</v>
       </c>
       <c r="B135" s="2" t="s">
@@ -9257,7 +9255,7 @@
       </c>
     </row>
     <row r="136" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="20">
+      <c r="A136" s="19">
         <v>135</v>
       </c>
       <c r="B136" s="2" t="s">
@@ -9292,7 +9290,7 @@
       </c>
     </row>
     <row r="137" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="20">
+      <c r="A137" s="19">
         <v>136</v>
       </c>
       <c r="B137" s="2" t="s">
@@ -9327,7 +9325,7 @@
       </c>
     </row>
     <row r="138" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="20">
+      <c r="A138" s="19">
         <v>137</v>
       </c>
       <c r="B138" s="2" t="s">
@@ -9362,7 +9360,7 @@
       </c>
     </row>
     <row r="139" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A139" s="20">
+      <c r="A139" s="19">
         <v>138</v>
       </c>
       <c r="B139" s="2" t="s">
@@ -9397,7 +9395,7 @@
       </c>
     </row>
     <row r="140" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A140" s="20">
+      <c r="A140" s="19">
         <v>139</v>
       </c>
       <c r="B140" s="2" t="s">
@@ -9432,7 +9430,7 @@
       </c>
     </row>
     <row r="141" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="20">
+      <c r="A141" s="19">
         <v>140</v>
       </c>
       <c r="B141" s="2" t="s">
@@ -9467,7 +9465,7 @@
       </c>
     </row>
     <row r="142" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A142" s="20">
+      <c r="A142" s="19">
         <v>141</v>
       </c>
       <c r="B142" s="2" t="s">
@@ -9502,7 +9500,7 @@
       </c>
     </row>
     <row r="143" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A143" s="20">
+      <c r="A143" s="19">
         <v>142</v>
       </c>
       <c r="B143" s="2" t="s">
@@ -9537,7 +9535,7 @@
       </c>
     </row>
     <row r="144" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A144" s="20">
+      <c r="A144" s="19">
         <v>143</v>
       </c>
       <c r="B144" s="2" t="s">
@@ -9572,7 +9570,7 @@
       </c>
     </row>
     <row r="145" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A145" s="20">
+      <c r="A145" s="19">
         <v>144</v>
       </c>
       <c r="B145" s="2" t="s">
@@ -9607,7 +9605,7 @@
       </c>
     </row>
     <row r="146" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A146" s="20">
+      <c r="A146" s="19">
         <v>145</v>
       </c>
       <c r="B146" s="2" t="s">
@@ -9642,7 +9640,7 @@
       </c>
     </row>
     <row r="147" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A147" s="20">
+      <c r="A147" s="19">
         <v>146</v>
       </c>
       <c r="B147" s="2" t="s">
@@ -9677,7 +9675,7 @@
       </c>
     </row>
     <row r="148" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A148" s="20">
+      <c r="A148" s="19">
         <v>147</v>
       </c>
       <c r="B148" s="2" t="s">
@@ -9712,7 +9710,7 @@
       </c>
     </row>
     <row r="149" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A149" s="20">
+      <c r="A149" s="19">
         <v>148</v>
       </c>
       <c r="B149" s="2" t="s">
@@ -9747,7 +9745,7 @@
       </c>
     </row>
     <row r="150" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A150" s="20">
+      <c r="A150" s="19">
         <v>149</v>
       </c>
       <c r="B150" s="2" t="s">
@@ -9782,7 +9780,7 @@
       </c>
     </row>
     <row r="151" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A151" s="20">
+      <c r="A151" s="19">
         <v>150</v>
       </c>
       <c r="B151" s="2" t="s">
@@ -9817,7 +9815,7 @@
       </c>
     </row>
     <row r="152" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A152" s="20">
+      <c r="A152" s="19">
         <v>151</v>
       </c>
       <c r="B152" s="2" t="s">
@@ -9849,7 +9847,7 @@
       </c>
     </row>
     <row r="153" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A153" s="20">
+      <c r="A153" s="19">
         <v>152</v>
       </c>
       <c r="B153" s="2" t="s">
@@ -9881,7 +9879,7 @@
       </c>
     </row>
     <row r="154" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A154" s="20">
+      <c r="A154" s="19">
         <v>153</v>
       </c>
       <c r="B154" s="2" t="s">
@@ -9913,7 +9911,7 @@
       </c>
     </row>
     <row r="155" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A155" s="20">
+      <c r="A155" s="19">
         <v>154</v>
       </c>
       <c r="B155" s="2" t="s">
@@ -9945,7 +9943,7 @@
       </c>
     </row>
     <row r="156" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A156" s="20">
+      <c r="A156" s="19">
         <v>155</v>
       </c>
       <c r="B156" s="2" t="s">
@@ -9977,7 +9975,7 @@
       </c>
     </row>
     <row r="157" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A157" s="20">
+      <c r="A157" s="19">
         <v>156</v>
       </c>
       <c r="B157" s="2" t="s">
@@ -10009,7 +10007,7 @@
       </c>
     </row>
     <row r="158" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A158" s="20">
+      <c r="A158" s="19">
         <v>157</v>
       </c>
       <c r="B158" s="2" t="s">
@@ -10041,7 +10039,7 @@
       </c>
     </row>
     <row r="159" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A159" s="20">
+      <c r="A159" s="19">
         <v>158</v>
       </c>
       <c r="B159" s="2" t="s">
@@ -10073,7 +10071,7 @@
       </c>
     </row>
     <row r="160" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A160" s="20">
+      <c r="A160" s="19">
         <v>159</v>
       </c>
       <c r="B160" s="2" t="s">
@@ -15654,9 +15652,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C1000"/>
+  <dimension ref="A1:F1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -15692,6 +15692,9 @@
       <c r="B3" s="6">
         <v>1600</v>
       </c>
+      <c r="C3">
+        <v>10</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -15918,22 +15921,24 @@
       </c>
     </row>
     <row r="32" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="42" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="44" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="45" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="46" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="47" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="48" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F33" s="20"/>
+    </row>
+    <row r="34" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="50" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="51" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -26081,7 +26086,7 @@
         <v>928</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -26095,7 +26100,7 @@
         <v>44484</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -26109,7 +26114,7 @@
         <v>44893</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -26123,7 +26128,7 @@
         <v>44877</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -26137,7 +26142,7 @@
         <v>43790</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -26151,7 +26156,7 @@
         <v>45213</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
@@ -26165,7 +26170,7 @@
         <v>44856</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
@@ -26179,7 +26184,7 @@
         <v>44864</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>3</v>
       </c>
@@ -26193,7 +26198,7 @@
         <v>44951</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>3</v>
       </c>
@@ -26207,7 +26212,7 @@
         <v>44812</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>3</v>
       </c>
@@ -26221,7 +26226,7 @@
         <v>44949</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>3</v>
       </c>
@@ -26235,7 +26240,7 @@
         <v>44855</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>3</v>
       </c>
@@ -26249,7 +26254,7 @@
         <v>45178</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>3</v>
       </c>
@@ -26263,7 +26268,7 @@
         <v>44952</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>3</v>
       </c>
@@ -26277,7 +26282,7 @@
         <v>937</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>3</v>
       </c>
@@ -26291,7 +26296,7 @@
         <v>45252</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>3</v>
       </c>
@@ -26305,7 +26310,7 @@
         <v>44808</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>3</v>
       </c>
@@ -26319,7 +26324,7 @@
         <v>44934</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>3</v>
       </c>
@@ -26333,7 +26338,7 @@
         <v>938</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>3</v>
       </c>
@@ -26347,7 +26352,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>3</v>
       </c>
@@ -26361,7 +26366,7 @@
         <v>44928</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>3</v>
       </c>
@@ -26375,7 +26380,7 @@
         <v>44814</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>24</v>
       </c>
@@ -26389,7 +26394,7 @@
         <v>44871</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>25</v>
       </c>
@@ -26403,7 +26408,7 @@
         <v>45179</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>26</v>
       </c>
@@ -26417,7 +26422,7 @@
         <v>43478</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>27</v>
       </c>
@@ -26431,7 +26436,7 @@
         <v>940</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>28</v>
       </c>
@@ -26445,7 +26450,7 @@
         <v>941</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>29</v>
       </c>
@@ -26459,7 +26464,7 @@
         <v>44938</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>30</v>
       </c>
@@ -26473,7 +26478,7 @@
         <v>942</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>31</v>
       </c>
@@ -26487,7 +26492,7 @@
         <v>43410</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>32</v>
       </c>
@@ -26501,7 +26506,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>3</v>
       </c>
@@ -26515,7 +26520,7 @@
         <v>44808</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>4</v>
       </c>
@@ -26529,7 +26534,7 @@
         <v>944</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>5</v>
       </c>
@@ -26543,7 +26548,7 @@
         <v>44842</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>6</v>
       </c>
@@ -26557,7 +26562,7 @@
         <v>43525</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>7</v>
       </c>
@@ -26571,7 +26576,7 @@
         <v>44875</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>8</v>
       </c>
@@ -26585,7 +26590,7 @@
         <v>44856</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>9</v>
       </c>
@@ -26599,7 +26604,7 @@
         <v>44928</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>10</v>
       </c>
@@ -26613,7 +26618,7 @@
         <v>44882</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>11</v>
       </c>
@@ -26627,7 +26632,7 @@
         <v>43747</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>12</v>
       </c>
@@ -26641,7 +26646,7 @@
         <v>945</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>13</v>
       </c>
@@ -26655,7 +26660,7 @@
         <v>44833</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>14</v>
       </c>
@@ -26669,7 +26674,7 @@
         <v>44877</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>15</v>
       </c>
@@ -26683,7 +26688,7 @@
         <v>946</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>16</v>
       </c>
@@ -26697,7 +26702,7 @@
         <v>43161</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>17</v>
       </c>
@@ -26711,7 +26716,7 @@
         <v>44893</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>18</v>
       </c>
@@ -26725,7 +26730,7 @@
         <v>44855</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>19</v>
       </c>
@@ -26739,7 +26744,7 @@
         <v>44947</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>20</v>
       </c>
@@ -26753,7 +26758,7 @@
         <v>44949</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>21</v>
       </c>
@@ -26767,7 +26772,7 @@
         <v>947</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>22</v>
       </c>
@@ -26781,7 +26786,7 @@
         <v>44890</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>23</v>
       </c>
@@ -26795,7 +26800,7 @@
         <v>44845</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>24</v>
       </c>
@@ -26809,7 +26814,7 @@
         <v>948</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>25</v>
       </c>
@@ -26823,7 +26828,7 @@
         <v>949</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>26</v>
       </c>
@@ -26837,7 +26842,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>27</v>
       </c>
@@ -26981,7 +26986,7 @@
       <c r="A66" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B66" s="20">
+      <c r="B66" s="19">
         <v>65</v>
       </c>
       <c r="C66" s="16">
@@ -27121,7 +27126,7 @@
       <c r="A76" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B76" s="20">
+      <c r="B76" s="19">
         <v>75</v>
       </c>
       <c r="C76" s="16">
@@ -27131,7 +27136,7 @@
         <v>44928</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>18</v>
       </c>
@@ -27142,7 +27147,7 @@
         <v>43728</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>19</v>
       </c>
@@ -27153,7 +27158,7 @@
         <v>43833</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>20</v>
       </c>
@@ -27164,7 +27169,7 @@
         <v>44301</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>21</v>
       </c>
@@ -27175,7 +27180,7 @@
         <v>43308</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>22</v>
       </c>
@@ -27186,7 +27191,7 @@
         <v>44873</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>23</v>
       </c>
@@ -27197,7 +27202,7 @@
         <v>43581</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>24</v>
       </c>
@@ -27208,7 +27213,7 @@
         <v>44083</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>25</v>
       </c>
@@ -27219,7 +27224,7 @@
         <v>44520</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>26</v>
       </c>
@@ -27230,7 +27235,7 @@
         <v>43134</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>27</v>
       </c>
@@ -27241,7 +27246,7 @@
         <v>44790</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>28</v>
       </c>
@@ -27252,7 +27257,7 @@
         <v>43488</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>29</v>
       </c>
@@ -27263,7 +27268,7 @@
         <v>43989</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>30</v>
       </c>
@@ -27274,7 +27279,7 @@
         <v>44427</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>31</v>
       </c>
@@ -27285,7 +27290,7 @@
         <v>43405</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>32</v>
       </c>
@@ -27296,7 +27301,7 @@
         <v>44634</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>3</v>
       </c>
@@ -27307,7 +27312,7 @@
         <v>43700</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>4</v>
       </c>
@@ -27318,7 +27323,7 @@
         <v>44202</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>5</v>
       </c>
@@ -27329,7 +27334,7 @@
         <v>44304</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>6</v>
       </c>
@@ -27340,7 +27345,7 @@
         <v>43281</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>7</v>
       </c>
@@ -27351,7 +27356,7 @@
         <v>44906</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>8</v>
       </c>
@@ -27362,7 +27367,7 @@
         <v>43494</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>9</v>
       </c>
@@ -27373,7 +27378,7 @@
         <v>43964</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>10</v>
       </c>
@@ -27384,7 +27389,7 @@
         <v>44463</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>11</v>
       </c>
@@ -27395,7 +27400,7 @@
         <v>43107</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>12</v>
       </c>
@@ -27406,7 +27411,7 @@
         <v>44762</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
         <v>13</v>
       </c>
@@ -27417,7 +27422,7 @@
         <v>43500</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
         <v>14</v>
       </c>
@@ -27428,7 +27433,7 @@
         <v>44031</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
         <v>15</v>
       </c>
@@ -27439,7 +27444,7 @@
         <v>44469</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
         <v>16</v>
       </c>
@@ -27450,7 +27455,7 @@
         <v>43445</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
         <v>17</v>
       </c>
@@ -27461,7 +27466,7 @@
         <v>44735</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
         <v>18</v>
       </c>
@@ -27472,7 +27477,7 @@
         <v>43777</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
         <v>19</v>
       </c>
@@ -27483,7 +27488,7 @@
         <v>43882</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
         <v>20</v>
       </c>
@@ -27494,7 +27499,7 @@
         <v>44350</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
         <v>21</v>
       </c>
@@ -27505,7 +27510,7 @@
         <v>43359</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
         <v>22</v>
       </c>
@@ -27516,7 +27521,7 @@
         <v>44588</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
         <v>23</v>
       </c>
@@ -27527,7 +27532,7 @@
         <v>43650</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
         <v>24</v>
       </c>
@@ -27538,7 +27543,7 @@
         <v>44152</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
         <v>25</v>
       </c>
@@ -27549,7 +27554,7 @@
         <v>936</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
         <v>26</v>
       </c>
@@ -27560,7 +27565,7 @@
         <v>43231</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
         <v>27</v>
       </c>
@@ -27571,7 +27576,7 @@
         <v>44827</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
         <v>28</v>
       </c>
@@ -27582,7 +27587,7 @@
         <v>43497</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
         <v>29</v>
       </c>
@@ -27593,7 +27598,7 @@
         <v>43998</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
         <v>30</v>
       </c>
@@ -27604,7 +27609,7 @@
         <v>44436</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
         <v>31</v>
       </c>
@@ -27615,7 +27620,7 @@
         <v>43414</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
         <v>32</v>
       </c>
@@ -27626,7 +27631,7 @@
         <v>44672</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
         <v>3</v>
       </c>
@@ -27637,7 +27642,7 @@
         <v>43743</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
         <v>4</v>
       </c>
@@ -27648,7 +27653,7 @@
         <v>44215</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
         <v>5</v>
       </c>
@@ -27659,7 +27664,7 @@
         <v>44287</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
         <v>6</v>
       </c>
@@ -27670,7 +27675,7 @@
         <v>43294</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
         <v>7</v>
       </c>
@@ -27681,7 +27686,7 @@
         <v>44892</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
         <v>8</v>
       </c>
@@ -27692,7 +27697,7 @@
         <v>43528</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
         <v>9</v>
       </c>
@@ -27703,7 +27708,7 @@
         <v>44029</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
         <v>10</v>
       </c>
@@ -27714,7 +27719,7 @@
         <v>44468</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
         <v>11</v>
       </c>
@@ -27725,7 +27730,7 @@
         <v>43112</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
         <v>12</v>
       </c>
@@ -27736,7 +27741,7 @@
         <v>44736</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
         <v>13</v>
       </c>
@@ -27747,7 +27752,7 @@
         <v>43505</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
         <v>14</v>
       </c>
@@ -27758,7 +27763,7 @@
         <v>44004</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
         <v>15</v>
       </c>
@@ -27769,7 +27774,7 @@
         <v>44443</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
         <v>16</v>
       </c>
@@ -27780,7 +27785,7 @@
         <v>43451</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
         <v>17</v>
       </c>
@@ -27791,7 +27796,7 @@
         <v>44772</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
         <v>18</v>
       </c>
@@ -27802,7 +27807,7 @@
         <v>43476</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
         <v>19</v>
       </c>
@@ -27813,7 +27818,7 @@
         <v>43945</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
         <v>20</v>
       </c>
@@ -27824,7 +27829,7 @@
         <v>44414</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
         <v>21</v>
       </c>
@@ -27835,7 +27840,7 @@
         <v>43422</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
         <v>22</v>
       </c>
@@ -27846,7 +27851,7 @@
         <v>44683</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
         <v>23</v>
       </c>
@@ -27857,7 +27862,7 @@
         <v>43757</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
         <v>24</v>
       </c>
@@ -27868,7 +27873,7 @@
         <v>44167</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
         <v>25</v>
       </c>
@@ -27879,7 +27884,7 @@
         <v>44634</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
         <v>26</v>
       </c>
@@ -27890,7 +27895,7 @@
         <v>43642</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
         <v>27</v>
       </c>
@@ -27901,7 +27906,7 @@
         <v>44144</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
         <v>28</v>
       </c>
@@ -27912,7 +27917,7 @@
         <v>44248</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
         <v>29</v>
       </c>
@@ -27923,7 +27928,7 @@
         <v>43224</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
         <v>30</v>
       </c>
@@ -27934,7 +27939,7 @@
         <v>44820</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
         <v>31</v>
       </c>
@@ -27945,7 +27950,7 @@
         <v>43527</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
         <v>32</v>
       </c>
@@ -27956,7 +27961,7 @@
         <v>44027</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
         <v>3</v>
       </c>
@@ -27967,7 +27972,7 @@
         <v>44435</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
         <v>4</v>
       </c>
@@ -27978,7 +27983,7 @@
         <v>43443</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
         <v>5</v>
       </c>
@@ -27989,7 +27994,7 @@
         <v>44672</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A155" s="2" t="s">
         <v>6</v>
       </c>
@@ -28000,7 +28005,7 @@
         <v>43744</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="s">
         <v>7</v>
       </c>
@@ -28011,7 +28016,7 @@
         <v>44215</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A157" s="2" t="s">
         <v>8</v>
       </c>
@@ -28022,7 +28027,7 @@
         <v>44287</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A158" s="2" t="s">
         <v>9</v>
       </c>
@@ -28033,7 +28038,7 @@
         <v>43294</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A159" s="2" t="s">
         <v>10</v>
       </c>
@@ -28044,7 +28049,7 @@
         <v>44892</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A160" s="2" t="s">
         <v>11</v>
       </c>
@@ -28055,7 +28060,7 @@
         <v>43533</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">
         <v>12</v>
       </c>
@@ -28066,7 +28071,7 @@
         <v>44034</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="s">
         <v>13</v>
       </c>
@@ -28077,7 +28082,7 @@
         <v>44442</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
         <v>14</v>
       </c>
@@ -28088,7 +28093,7 @@
         <v>43450</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
         <v>15</v>
       </c>
@@ -28099,7 +28104,7 @@
         <v>44589</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A165" s="2" t="s">
         <v>16</v>
       </c>
@@ -28110,7 +28115,7 @@
         <v>43628</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A166" s="2" t="s">
         <v>17</v>
       </c>
@@ -28121,7 +28126,7 @@
         <v>44129</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="s">
         <v>18</v>
       </c>
@@ -28132,7 +28137,7 @@
         <v>44203</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A168" s="2" t="s">
         <v>19</v>
       </c>
@@ -28143,7 +28148,7 @@
         <v>43209</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A169" s="2" t="s">
         <v>20</v>
       </c>
@@ -28154,7 +28159,7 @@
         <v>44804</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
         <v>21</v>
       </c>
@@ -28165,7 +28170,7 @@
         <v>43509</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
         <v>22</v>
       </c>
@@ -28176,7 +28181,7 @@
         <v>44009</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="s">
         <v>23</v>
       </c>
@@ -28187,7 +28192,7 @@
         <v>44448</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A173" s="2" t="s">
         <v>24</v>
       </c>
@@ -28198,7 +28203,7 @@
         <v>43456</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A174" s="2" t="s">
         <v>25</v>
       </c>
@@ -28209,7 +28214,7 @@
         <v>44685</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A175" s="2" t="s">
         <v>26</v>
       </c>
@@ -28220,7 +28225,7 @@
         <v>43756</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A176" s="2" t="s">
         <v>27</v>
       </c>
@@ -28231,7 +28236,7 @@
         <v>44197</v>
       </c>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A177" s="2" t="s">
         <v>28</v>
       </c>
@@ -28242,7 +28247,7 @@
         <v>44665</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A178" s="2" t="s">
         <v>29</v>
       </c>
@@ -28253,7 +28258,7 @@
         <v>43672</v>
       </c>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A179" s="2" t="s">
         <v>30</v>
       </c>
@@ -28264,7 +28269,7 @@
         <v>44173</v>
       </c>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A180" s="2" t="s">
         <v>31</v>
       </c>
@@ -28275,7 +28280,7 @@
         <v>44247</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
         <v>32</v>
       </c>
@@ -28286,7 +28291,7 @@
         <v>43253</v>
       </c>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
         <v>3</v>
       </c>
@@ -28297,7 +28302,7 @@
         <v>44879</v>
       </c>
     </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
         <v>4</v>
       </c>
@@ -28308,7 +28313,7 @@
         <v>43521</v>
       </c>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A184" s="2" t="s">
         <v>5</v>
       </c>
@@ -28319,7 +28324,7 @@
         <v>44020</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A185" s="2" t="s">
         <v>6</v>
       </c>
@@ -28330,7 +28335,7 @@
         <v>44459</v>
       </c>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A186" s="2" t="s">
         <v>7</v>
       </c>
@@ -28341,7 +28346,7 @@
         <v>43103</v>
       </c>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A187" s="2" t="s">
         <v>8</v>
       </c>
@@ -28352,7 +28357,7 @@
         <v>44697</v>
       </c>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A188" s="2" t="s">
         <v>9</v>
       </c>
@@ -28363,7 +28368,7 @@
         <v>43737</v>
       </c>
     </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A189" s="2" t="s">
         <v>10</v>
       </c>
@@ -28374,7 +28379,7 @@
         <v>44207</v>
       </c>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A190" s="2" t="s">
         <v>11</v>
       </c>
@@ -28385,7 +28390,7 @@
         <v>44309</v>
       </c>
     </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A191" s="2" t="s">
         <v>12</v>
       </c>
@@ -28396,7 +28401,7 @@
         <v>43317</v>
       </c>
     </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A192" s="2" t="s">
         <v>13</v>
       </c>
@@ -28407,7 +28412,7 @@
         <v>44882</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A193" s="2" t="s">
         <v>14</v>
       </c>
@@ -28418,7 +28423,7 @@
         <v>43526</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A194" s="2" t="s">
         <v>15</v>
       </c>
@@ -28429,7 +28434,7 @@
         <v>44027</v>
       </c>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A195" s="2" t="s">
         <v>16</v>
       </c>
@@ -28440,7 +28445,7 @@
         <v>44435</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A196" s="2" t="s">
         <v>17</v>
       </c>
@@ -28451,7 +28456,7 @@
         <v>43443</v>
       </c>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A197" s="2" t="s">
         <v>18</v>
       </c>
@@ -28462,7 +28467,7 @@
         <v>44672</v>
       </c>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A198" s="2" t="s">
         <v>19</v>
       </c>
@@ -28473,7 +28478,7 @@
         <v>43743</v>
       </c>
     </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A199" s="2" t="s">
         <v>20</v>
       </c>
@@ -28484,7 +28489,7 @@
         <v>44214</v>
       </c>
     </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A200" s="2" t="s">
         <v>21</v>
       </c>
@@ -28495,7 +28500,7 @@
         <v>44287</v>
       </c>
     </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A201" s="2" t="s">
         <v>22</v>
       </c>
@@ -28506,7 +28511,7 @@
         <v>43294</v>
       </c>
     </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A202" s="2" t="s">
         <v>23</v>
       </c>
@@ -28517,7 +28522,7 @@
         <v>44892</v>
       </c>
     </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A203" s="2" t="s">
         <v>24</v>
       </c>
@@ -28528,7 +28533,7 @@
         <v>43533</v>
       </c>
     </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A204" s="2" t="s">
         <v>25</v>
       </c>
@@ -28539,7 +28544,7 @@
         <v>44034</v>
       </c>
     </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A205" s="2" t="s">
         <v>26</v>
       </c>
@@ -28550,7 +28555,7 @@
         <v>44442</v>
       </c>
     </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A206" s="2" t="s">
         <v>27</v>
       </c>
@@ -28561,7 +28566,7 @@
         <v>43450</v>
       </c>
     </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A207" s="2" t="s">
         <v>28</v>
       </c>
@@ -28572,7 +28577,7 @@
         <v>44589</v>
       </c>
     </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A208" s="2" t="s">
         <v>29</v>
       </c>
@@ -28583,7 +28588,7 @@
         <v>43628</v>
       </c>
     </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A209" s="2" t="s">
         <v>30</v>
       </c>
@@ -28594,7 +28599,7 @@
         <v>44129</v>
       </c>
     </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A210" s="2" t="s">
         <v>31</v>
       </c>
@@ -28605,7 +28610,7 @@
         <v>44203</v>
       </c>
     </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A211" s="2" t="s">
         <v>32</v>
       </c>
@@ -28616,7 +28621,7 @@
         <v>43209</v>
       </c>
     </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A212" s="2" t="s">
         <v>3</v>
       </c>
@@ -28627,7 +28632,7 @@
         <v>44804</v>
       </c>
     </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A213" s="2" t="s">
         <v>4</v>
       </c>
@@ -28638,7 +28643,7 @@
         <v>43509</v>
       </c>
     </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A214" s="2" t="s">
         <v>5</v>
       </c>
@@ -28649,7 +28654,7 @@
         <v>44009</v>
       </c>
     </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A215" s="2" t="s">
         <v>6</v>
       </c>
@@ -28660,7 +28665,7 @@
         <v>44448</v>
       </c>
     </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A216" s="2" t="s">
         <v>7</v>
       </c>
@@ -28671,7 +28676,7 @@
         <v>43456</v>
       </c>
     </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A217" s="2" t="s">
         <v>8</v>
       </c>
@@ -28682,7 +28687,7 @@
         <v>44685</v>
       </c>
     </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A218" s="2" t="s">
         <v>9</v>
       </c>
@@ -28693,7 +28698,7 @@
         <v>43756</v>
       </c>
     </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A219" s="2" t="s">
         <v>10</v>
       </c>
@@ -28704,7 +28709,7 @@
         <v>44197</v>
       </c>
     </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A220" s="2" t="s">
         <v>11</v>
       </c>
@@ -28715,7 +28720,7 @@
         <v>44665</v>
       </c>
     </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A221" s="2" t="s">
         <v>12</v>
       </c>
@@ -28726,7 +28731,7 @@
         <v>43672</v>
       </c>
     </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A222" s="2" t="s">
         <v>13</v>
       </c>
@@ -28737,7 +28742,7 @@
         <v>44173</v>
       </c>
     </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A223" s="2" t="s">
         <v>14</v>
       </c>
@@ -28748,7 +28753,7 @@
         <v>44247</v>
       </c>
     </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A224" s="2" t="s">
         <v>15</v>
       </c>
@@ -28759,7 +28764,7 @@
         <v>43253</v>
       </c>
     </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A225" s="2" t="s">
         <v>16</v>
       </c>
@@ -28770,7 +28775,7 @@
         <v>44879</v>
       </c>
     </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A226" s="2" t="s">
         <v>17</v>
       </c>
@@ -28781,7 +28786,7 @@
         <v>43521</v>
       </c>
     </row>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A227" s="2" t="s">
         <v>18</v>
       </c>
@@ -28792,7 +28797,7 @@
         <v>44020</v>
       </c>
     </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A228" s="2" t="s">
         <v>19</v>
       </c>
@@ -28803,7 +28808,7 @@
         <v>44459</v>
       </c>
     </row>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A229" s="2" t="s">
         <v>20</v>
       </c>
@@ -28814,7 +28819,7 @@
         <v>43103</v>
       </c>
     </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A230" s="2" t="s">
         <v>21</v>
       </c>
@@ -28825,7 +28830,7 @@
         <v>44697</v>
       </c>
     </row>
-    <row r="231" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A231" s="2" t="s">
         <v>22</v>
       </c>
@@ -28836,7 +28841,7 @@
         <v>43737</v>
       </c>
     </row>
-    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A232" s="2" t="s">
         <v>23</v>
       </c>
@@ -28847,7 +28852,7 @@
         <v>44207</v>
       </c>
     </row>
-    <row r="233" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A233" s="2" t="s">
         <v>24</v>
       </c>
@@ -28858,7 +28863,7 @@
         <v>44309</v>
       </c>
     </row>
-    <row r="234" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A234" s="2" t="s">
         <v>25</v>
       </c>
@@ -28869,7 +28874,7 @@
         <v>43317</v>
       </c>
     </row>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A235" s="2" t="s">
         <v>26</v>
       </c>
@@ -28880,7 +28885,7 @@
         <v>44882</v>
       </c>
     </row>
-    <row r="236" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A236" s="2" t="s">
         <v>27</v>
       </c>
@@ -28891,7 +28896,7 @@
         <v>43526</v>
       </c>
     </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A237" s="2" t="s">
         <v>28</v>
       </c>
@@ -28902,7 +28907,7 @@
         <v>44027</v>
       </c>
     </row>
-    <row r="238" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A238" s="2" t="s">
         <v>29</v>
       </c>
@@ -28913,7 +28918,7 @@
         <v>44435</v>
       </c>
     </row>
-    <row r="239" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A239" s="2" t="s">
         <v>30</v>
       </c>
@@ -28924,7 +28929,7 @@
         <v>43443</v>
       </c>
     </row>
-    <row r="240" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A240" s="2" t="s">
         <v>31</v>
       </c>
@@ -28935,7 +28940,7 @@
         <v>44672</v>
       </c>
     </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A241" s="2" t="s">
         <v>32</v>
       </c>
@@ -28946,7 +28951,7 @@
         <v>43743</v>
       </c>
     </row>
-    <row r="242" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A242" s="2" t="s">
         <v>3</v>
       </c>
@@ -28957,7 +28962,7 @@
         <v>44214</v>
       </c>
     </row>
-    <row r="243" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A243" s="2" t="s">
         <v>4</v>
       </c>
@@ -28968,7 +28973,7 @@
         <v>44287</v>
       </c>
     </row>
-    <row r="244" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A244" s="2" t="s">
         <v>5</v>
       </c>
@@ -28979,7 +28984,7 @@
         <v>43294</v>
       </c>
     </row>
-    <row r="245" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A245" s="2" t="s">
         <v>6</v>
       </c>
@@ -28990,7 +28995,7 @@
         <v>44892</v>
       </c>
     </row>
-    <row r="246" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A246" s="2" t="s">
         <v>7</v>
       </c>
@@ -29001,7 +29006,7 @@
         <v>43533</v>
       </c>
     </row>
-    <row r="247" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A247" s="2" t="s">
         <v>8</v>
       </c>
@@ -29012,7 +29017,7 @@
         <v>44034</v>
       </c>
     </row>
-    <row r="248" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A248" s="2" t="s">
         <v>9</v>
       </c>
@@ -29023,7 +29028,7 @@
         <v>44442</v>
       </c>
     </row>
-    <row r="249" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A249" s="2" t="s">
         <v>10</v>
       </c>
@@ -29034,7 +29039,7 @@
         <v>43450</v>
       </c>
     </row>
-    <row r="250" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A250" s="2" t="s">
         <v>11</v>
       </c>
@@ -29045,7 +29050,7 @@
         <v>44589</v>
       </c>
     </row>
-    <row r="251" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A251" s="2" t="s">
         <v>12</v>
       </c>
@@ -29056,7 +29061,7 @@
         <v>43628</v>
       </c>
     </row>
-    <row r="252" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A252" s="2" t="s">
         <v>13</v>
       </c>
@@ -29067,7 +29072,7 @@
         <v>44129</v>
       </c>
     </row>
-    <row r="253" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A253" s="2" t="s">
         <v>14</v>
       </c>
@@ -29078,7 +29083,7 @@
         <v>44203</v>
       </c>
     </row>
-    <row r="254" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A254" s="2" t="s">
         <v>15</v>
       </c>
@@ -29089,7 +29094,7 @@
         <v>43209</v>
       </c>
     </row>
-    <row r="255" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A255" s="2" t="s">
         <v>16</v>
       </c>
@@ -29100,7 +29105,7 @@
         <v>44804</v>
       </c>
     </row>
-    <row r="256" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A256" s="2" t="s">
         <v>17</v>
       </c>
@@ -29111,7 +29116,7 @@
         <v>43509</v>
       </c>
     </row>
-    <row r="257" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A257" s="2" t="s">
         <v>18</v>
       </c>
@@ -29122,7 +29127,7 @@
         <v>44009</v>
       </c>
     </row>
-    <row r="258" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A258" s="2" t="s">
         <v>19</v>
       </c>
@@ -29133,7 +29138,7 @@
         <v>44448</v>
       </c>
     </row>
-    <row r="259" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A259" s="2" t="s">
         <v>20</v>
       </c>
@@ -29144,7 +29149,7 @@
         <v>43456</v>
       </c>
     </row>
-    <row r="260" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A260" s="2" t="s">
         <v>21</v>
       </c>
@@ -29155,7 +29160,7 @@
         <v>44685</v>
       </c>
     </row>
-    <row r="261" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A261" s="2" t="s">
         <v>22</v>
       </c>
@@ -29166,7 +29171,7 @@
         <v>43756</v>
       </c>
     </row>
-    <row r="262" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A262" s="2" t="s">
         <v>23</v>
       </c>
@@ -29177,7 +29182,7 @@
         <v>44197</v>
       </c>
     </row>
-    <row r="263" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A263" s="2" t="s">
         <v>24</v>
       </c>
@@ -29188,7 +29193,7 @@
         <v>44665</v>
       </c>
     </row>
-    <row r="264" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A264" s="2" t="s">
         <v>25</v>
       </c>
@@ -29199,7 +29204,7 @@
         <v>43672</v>
       </c>
     </row>
-    <row r="265" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A265" s="2" t="s">
         <v>26</v>
       </c>
@@ -29210,7 +29215,7 @@
         <v>44173</v>
       </c>
     </row>
-    <row r="266" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A266" s="2" t="s">
         <v>27</v>
       </c>
@@ -29221,7 +29226,7 @@
         <v>44247</v>
       </c>
     </row>
-    <row r="267" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A267" s="2" t="s">
         <v>28</v>
       </c>
@@ -29232,7 +29237,7 @@
         <v>43253</v>
       </c>
     </row>
-    <row r="268" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A268" s="2" t="s">
         <v>29</v>
       </c>
@@ -29243,7 +29248,7 @@
         <v>44879</v>
       </c>
     </row>
-    <row r="269" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A269" s="2" t="s">
         <v>30</v>
       </c>
@@ -29254,7 +29259,7 @@
         <v>43521</v>
       </c>
     </row>
-    <row r="270" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A270" s="2" t="s">
         <v>31</v>
       </c>
@@ -29265,7 +29270,7 @@
         <v>44020</v>
       </c>
     </row>
-    <row r="271" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A271" s="2" t="s">
         <v>32</v>
       </c>
@@ -29276,7 +29281,7 @@
         <v>44459</v>
       </c>
     </row>
-    <row r="272" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A272" s="2" t="s">
         <v>3</v>
       </c>
@@ -29287,7 +29292,7 @@
         <v>43103</v>
       </c>
     </row>
-    <row r="273" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A273" s="2" t="s">
         <v>4</v>
       </c>
@@ -29298,7 +29303,7 @@
         <v>44697</v>
       </c>
     </row>
-    <row r="274" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A274" s="2" t="s">
         <v>5</v>
       </c>
@@ -29309,7 +29314,7 @@
         <v>43737</v>
       </c>
     </row>
-    <row r="275" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A275" s="2" t="s">
         <v>6</v>
       </c>
@@ -29320,7 +29325,7 @@
         <v>44207</v>
       </c>
     </row>
-    <row r="276" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A276" s="2" t="s">
         <v>7</v>
       </c>
@@ -29331,7 +29336,7 @@
         <v>44309</v>
       </c>
     </row>
-    <row r="277" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A277" s="2" t="s">
         <v>8</v>
       </c>
@@ -29342,7 +29347,7 @@
         <v>43317</v>
       </c>
     </row>
-    <row r="278" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A278" s="2" t="s">
         <v>9</v>
       </c>
@@ -29353,7 +29358,7 @@
         <v>44882</v>
       </c>
     </row>
-    <row r="279" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A279" s="2" t="s">
         <v>10</v>
       </c>
@@ -29364,7 +29369,7 @@
         <v>43526</v>
       </c>
     </row>
-    <row r="280" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A280" s="2" t="s">
         <v>11</v>
       </c>
@@ -29375,7 +29380,7 @@
         <v>44027</v>
       </c>
     </row>
-    <row r="281" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A281" s="2" t="s">
         <v>12</v>
       </c>
@@ -29386,7 +29391,7 @@
         <v>44435</v>
       </c>
     </row>
-    <row r="282" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A282" s="2" t="s">
         <v>13</v>
       </c>
@@ -29397,7 +29402,7 @@
         <v>43443</v>
       </c>
     </row>
-    <row r="283" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A283" s="2" t="s">
         <v>14</v>
       </c>
@@ -29408,7 +29413,7 @@
         <v>44672</v>
       </c>
     </row>
-    <row r="284" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A284" s="2" t="s">
         <v>15</v>
       </c>
@@ -29419,7 +29424,7 @@
         <v>43743</v>
       </c>
     </row>
-    <row r="285" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A285" s="2" t="s">
         <v>16</v>
       </c>
@@ -29430,7 +29435,7 @@
         <v>44214</v>
       </c>
     </row>
-    <row r="286" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A286" s="2" t="s">
         <v>17</v>
       </c>
@@ -29441,7 +29446,7 @@
         <v>44287</v>
       </c>
     </row>
-    <row r="287" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A287" s="2" t="s">
         <v>18</v>
       </c>
@@ -29452,7 +29457,7 @@
         <v>43294</v>
       </c>
     </row>
-    <row r="288" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A288" s="2" t="s">
         <v>19</v>
       </c>
@@ -29463,7 +29468,7 @@
         <v>44892</v>
       </c>
     </row>
-    <row r="289" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A289" s="2" t="s">
         <v>20</v>
       </c>
@@ -29474,7 +29479,7 @@
         <v>43533</v>
       </c>
     </row>
-    <row r="290" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A290" s="2" t="s">
         <v>21</v>
       </c>
@@ -29485,7 +29490,7 @@
         <v>43370</v>
       </c>
     </row>
-    <row r="291" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A291" s="2" t="s">
         <v>22</v>
       </c>
@@ -29496,7 +29501,7 @@
         <v>44756</v>
       </c>
     </row>
-    <row r="292" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A292" s="2" t="s">
         <v>23</v>
       </c>
@@ -29507,7 +29512,7 @@
         <v>43787</v>
       </c>
     </row>
-    <row r="293" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A293" s="2" t="s">
         <v>24</v>
       </c>
@@ -29518,7 +29523,7 @@
         <v>43984</v>
       </c>
     </row>
-    <row r="294" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A294" s="2" t="s">
         <v>25</v>
       </c>
@@ -29529,7 +29534,7 @@
         <v>44448</v>
       </c>
     </row>
-    <row r="295" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A295" s="2" t="s">
         <v>26</v>
       </c>
@@ -29540,7 +29545,7 @@
         <v>954</v>
       </c>
     </row>
-    <row r="296" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A296" s="2" t="s">
         <v>27</v>
       </c>
@@ -29551,7 +29556,7 @@
         <v>44839</v>
       </c>
     </row>
-    <row r="297" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A297" s="2" t="s">
         <v>28</v>
       </c>
@@ -29562,7 +29567,7 @@
         <v>955</v>
       </c>
     </row>
-    <row r="298" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A298" s="2" t="s">
         <v>29</v>
       </c>
@@ -29573,7 +29578,7 @@
         <v>43919</v>
       </c>
     </row>
-    <row r="299" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A299" s="2" t="s">
         <v>30</v>
       </c>
@@ -29584,7 +29589,7 @@
         <v>44481</v>
       </c>
     </row>
-    <row r="300" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A300" s="2" t="s">
         <v>31</v>
       </c>
@@ -29595,7 +29600,7 @@
         <v>956</v>
       </c>
     </row>
-    <row r="301" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A301" s="2" t="s">
         <v>32</v>
       </c>
@@ -29625,7 +29630,7 @@
       <c r="B303" s="1">
         <v>65</v>
       </c>
-      <c r="C303" s="19">
+      <c r="C303" s="18">
         <v>45002</v>
       </c>
       <c r="D303" s="12"/>
@@ -31348,7 +31353,7 @@
       <c r="B28" s="14">
         <v>2</v>
       </c>
-      <c r="C28" s="18">
+      <c r="C28" s="12">
         <v>45208</v>
       </c>
       <c r="D28" s="5">
@@ -31362,7 +31367,7 @@
       <c r="B29" s="14">
         <v>4</v>
       </c>
-      <c r="C29" s="18">
+      <c r="C29" s="12">
         <v>45002</v>
       </c>
       <c r="D29" s="5">

</xml_diff>